<commit_message>
add web sort operation
</commit_message>
<xml_diff>
--- a/tests/fixtures/inventory_items.xlsx
+++ b/tests/fixtures/inventory_items.xlsx
@@ -178,6 +178,9 @@
     <t xml:space="preserve">TEST INVENTORY ITEM 1</t>
   </si>
   <si>
+    <t xml:space="preserve">Missing Web Sortcode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Uno</t>
   </si>
   <si>
@@ -193,42 +196,42 @@
     <t xml:space="preserve">M</t>
   </si>
   <si>
+    <t xml:space="preserve">Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EACH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12340002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">110002</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEST INVENTORY ITEM 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Has Min Stock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">1001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EACH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01A1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12340002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">110002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEST INVENTORY ITEM 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Has Min Stock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02</t>
-  </si>
-  <si>
     <t xml:space="preserve">1002</t>
   </si>
   <si>
@@ -256,9 +259,6 @@
     <t xml:space="preserve">03</t>
   </si>
   <si>
-    <t xml:space="preserve">Y</t>
-  </si>
-  <si>
     <t xml:space="preserve">1003</t>
   </si>
   <si>
@@ -385,7 +385,7 @@
     <t xml:space="preserve">TEST INVENTORY ITEM 8</t>
   </si>
   <si>
-    <t xml:space="preserve">Missing web sortcode</t>
+    <t xml:space="preserve">Not web sortable</t>
   </si>
   <si>
     <t xml:space="preserve">Ocho</t>
@@ -456,7 +456,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY\ HH:MM"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy\ hh:mm"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -604,12 +604,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -675,17 +675,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AV11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M2" activeCellId="0" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="16.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.91"/>
@@ -700,7 +700,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="16.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="6.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="25.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="20.76"/>
@@ -708,21 +708,21 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="13.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="6.73"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="1" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="10.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="18.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="14.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="11.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="19.58"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="11.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="12.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="19.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="6.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="1" width="9.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="1" width="26.6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="40" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="49" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="49" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -884,30 +884,30 @@
       <c r="D2" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>52</v>
+      </c>
       <c r="F2" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J2" s="3"/>
       <c r="K2" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L2" s="3"/>
       <c r="M2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="N2" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="N2" s="3"/>
       <c r="O2" s="3"/>
       <c r="P2" s="3" t="s">
         <v>59</v>
@@ -1018,25 +1018,25 @@
         <v>68</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J3" s="3"/>
       <c r="K3" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L3" s="3"/>
       <c r="M3" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O3" s="3"/>
       <c r="P3" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q3" s="4" t="n">
         <v>1</v>
@@ -1091,7 +1091,7 @@
       </c>
       <c r="AL3" s="3"/>
       <c r="AM3" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="AN3" s="4" t="n">
         <v>3</v>
@@ -1123,39 +1123,39 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J4" s="3"/>
       <c r="K4" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L4" s="3"/>
       <c r="M4" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>79</v>
@@ -1270,18 +1270,18 @@
         <v>86</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="L5" s="3"/>
       <c r="M5" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>87</v>
@@ -1398,10 +1398,10 @@
         <v>95</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -1409,7 +1409,7 @@
         <v>96</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>97</v>
@@ -1525,13 +1525,13 @@
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N7" s="3" t="s">
         <v>106</v>
@@ -1645,13 +1645,13 @@
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N8" s="3" t="s">
         <v>114</v>
@@ -1769,13 +1769,13 @@
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
@@ -1889,13 +1889,13 @@
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="N10" s="3" t="s">
         <v>131</v>
@@ -2011,7 +2011,7 @@
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>139</v>
@@ -2019,7 +2019,7 @@
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="M11" s="3" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="N11" s="3" t="s">
         <v>140</v>

</xml_diff>